<commit_message>
Stopppoint: Prepare to merge back to development
Prepare for Standup demo
</commit_message>
<xml_diff>
--- a/VibeTrack/src/DataBase/Venues.xlsx
+++ b/VibeTrack/src/DataBase/Venues.xlsx
@@ -4,12 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="84" windowWidth="19140" windowHeight="8496"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19140" windowHeight="8490"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -263,9 +261,6 @@
     <t>cheathamstreet</t>
   </si>
   <si>
-    <t>chimy</t>
-  </si>
-  <si>
     <t>codys</t>
   </si>
   <si>
@@ -276,6 +271,9 @@
   </si>
   <si>
     <t>evo</t>
+  </si>
+  <si>
+    <t>chimys</t>
   </si>
 </sst>
 </file>
@@ -675,23 +673,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="55" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="55" defaultRowHeight="39" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="30.77734375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="51.6640625" customWidth="1"/>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="51.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
     <col min="9" max="9" width="55" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="23.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>50</v>
       </c>
@@ -950,7 +948,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>41</v>
@@ -977,12 +975,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>42</v>
@@ -1014,7 +1012,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>43</v>
@@ -1046,7 +1044,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>44</v>
@@ -1076,7 +1074,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>45</v>
@@ -1120,28 +1118,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>